<commit_message>
More of JSR fixed
Need to figure out how to set desired default values at particular memory locations.
</commit_message>
<xml_diff>
--- a/test4-desiredresults.xlsx
+++ b/test4-desiredresults.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="86">
   <si>
     <t xml:space="preserve">start</t>
   </si>
@@ -49,7 +49,7 @@
     <t xml:space="preserve">[600] = 650</t>
   </si>
   <si>
-    <t xml:space="preserve">[FC] = </t>
+    <t xml:space="preserve">[FC] = 400</t>
   </si>
   <si>
     <t xml:space="preserve">EXG Test</t>
@@ -118,9 +118,18 @@
     <t xml:space="preserve">FCB0</t>
   </si>
   <si>
+    <t xml:space="preserve">addr</t>
+  </si>
+  <si>
+    <t xml:space="preserve">instr</t>
+  </si>
+  <si>
     <t xml:space="preserve">NEG [n]</t>
   </si>
   <si>
+    <t xml:space="preserve">FC</t>
+  </si>
+  <si>
     <t xml:space="preserve">5C</t>
   </si>
   <si>
@@ -130,6 +139,9 @@
     <t xml:space="preserve">n + X -&gt; X</t>
   </si>
   <si>
+    <t xml:space="preserve">10C</t>
+  </si>
+  <si>
     <t xml:space="preserve">[n] + [X] -&gt; [X]</t>
   </si>
   <si>
@@ -232,10 +244,40 @@
     <t xml:space="preserve">JSR Test</t>
   </si>
   <si>
-    <t xml:space="preserve">[SP] – 1 → SP, [Pcupd] → [SP], EAdst → PC</t>
-  </si>
-  <si>
-    <t xml:space="preserve">FC</t>
+    <t xml:space="preserve">[n] → AC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">JSR [AC]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FF04</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RTS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">n → [AC]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">JSR [[AC]]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">JSR (AC)+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FF03</t>
+  </si>
+  <si>
+    <t xml:space="preserve">JSR -(AC)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">JSR [n+AC]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">JSR [n]</t>
   </si>
 </sst>
 </file>
@@ -672,7 +714,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="16" xfId="21" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="16" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -780,15 +822,16 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:R68"/>
+  <dimension ref="A1:R87"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A36" activeCellId="0" sqref="A36"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A45" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D77" activeCellId="0" sqref="D77"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5390625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="22.15"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="10.51"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1171,13 +1214,19 @@
       <c r="I17" s="13"/>
       <c r="J17" s="14"/>
       <c r="K17" s="15"/>
+      <c r="N17" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="O17" s="0" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="9" t="n">
         <v>450</v>
       </c>
       <c r="B18" s="10" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="C18" s="11"/>
       <c r="D18" s="12"/>
@@ -1193,6 +1242,12 @@
       </c>
       <c r="J18" s="14"/>
       <c r="K18" s="15"/>
+      <c r="N18" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="O18" s="0" t="n">
+        <v>400</v>
+      </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="9" t="n">
@@ -1213,6 +1268,12 @@
       <c r="I19" s="13"/>
       <c r="J19" s="14"/>
       <c r="K19" s="15"/>
+      <c r="N19" s="0" t="n">
+        <v>100</v>
+      </c>
+      <c r="O19" s="0" t="n">
+        <v>400</v>
+      </c>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="9" t="n">
@@ -1227,17 +1288,23 @@
       <c r="D20" s="12"/>
       <c r="E20" s="13"/>
       <c r="F20" s="14" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="G20" s="11"/>
       <c r="H20" s="12"/>
       <c r="I20" s="13"/>
       <c r="J20" s="14"/>
       <c r="K20" s="15"/>
+      <c r="N20" s="0" t="n">
+        <v>104</v>
+      </c>
+      <c r="O20" s="0" t="n">
+        <v>80</v>
+      </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="25" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="B21" s="26"/>
       <c r="C21" s="26"/>
@@ -1255,7 +1322,7 @@
         <v>1601</v>
       </c>
       <c r="B22" s="10" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="C22" s="11"/>
       <c r="D22" s="12" t="n">
@@ -1270,6 +1337,12 @@
       <c r="I22" s="13"/>
       <c r="J22" s="14"/>
       <c r="K22" s="15"/>
+      <c r="N22" s="0" t="n">
+        <v>108</v>
+      </c>
+      <c r="O22" s="0" t="n">
+        <v>400</v>
+      </c>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="9" t="n">
@@ -1290,13 +1363,19 @@
       <c r="I23" s="13"/>
       <c r="J23" s="14"/>
       <c r="K23" s="15"/>
+      <c r="N23" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="O23" s="0" t="n">
+        <v>80</v>
+      </c>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="9" t="n">
         <v>1511</v>
       </c>
       <c r="B24" s="10" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="C24" s="11"/>
       <c r="D24" s="12"/>
@@ -1308,7 +1387,7 @@
       <c r="G24" s="11"/>
       <c r="H24" s="12"/>
       <c r="I24" s="16" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="J24" s="32"/>
       <c r="K24" s="15"/>
@@ -1324,7 +1403,7 @@
       <c r="D25" s="12"/>
       <c r="E25" s="13"/>
       <c r="F25" s="14" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="G25" s="11"/>
       <c r="H25" s="12"/>
@@ -1337,7 +1416,7 @@
         <v>1242</v>
       </c>
       <c r="B26" s="10" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="C26" s="33" t="n">
         <v>2</v>
@@ -1380,7 +1459,7 @@
         <v>1633</v>
       </c>
       <c r="B28" s="10" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="C28" s="11"/>
       <c r="D28" s="12"/>
@@ -1408,7 +1487,7 @@
       <c r="D29" s="12"/>
       <c r="E29" s="13"/>
       <c r="F29" s="14" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="G29" s="11"/>
       <c r="H29" s="12"/>
@@ -1418,7 +1497,7 @@
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="25" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="B30" s="26"/>
       <c r="C30" s="26"/>
@@ -1436,7 +1515,7 @@
         <v>2600</v>
       </c>
       <c r="B31" s="10" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="C31" s="11" t="n">
         <v>0</v>
@@ -1460,7 +1539,7 @@
         <v>12</v>
       </c>
       <c r="C32" s="11" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="D32" s="12"/>
       <c r="E32" s="13"/>
@@ -1479,7 +1558,7 @@
         <v>2511</v>
       </c>
       <c r="B33" s="10" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="C33" s="11"/>
       <c r="D33" s="12"/>
@@ -1505,7 +1584,7 @@
       <c r="D34" s="12"/>
       <c r="E34" s="13"/>
       <c r="F34" s="14" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="G34" s="11"/>
       <c r="H34" s="12"/>
@@ -1518,7 +1597,7 @@
         <v>2249</v>
       </c>
       <c r="B35" s="10" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="C35" s="11"/>
       <c r="D35" s="12"/>
@@ -1532,7 +1611,7 @@
       <c r="H35" s="12"/>
       <c r="I35" s="13"/>
       <c r="J35" s="32" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="K35" s="15"/>
     </row>
@@ -1561,12 +1640,12 @@
         <v>2633</v>
       </c>
       <c r="B37" s="10" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="C37" s="11"/>
       <c r="D37" s="12"/>
       <c r="E37" s="16" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="F37" s="14" t="n">
         <f aca="false">F36+4</f>
@@ -1589,7 +1668,7 @@
       <c r="D38" s="12"/>
       <c r="E38" s="13"/>
       <c r="F38" s="14" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="G38" s="11"/>
       <c r="H38" s="12"/>
@@ -1599,7 +1678,7 @@
     </row>
     <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="25" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="B39" s="26"/>
       <c r="C39" s="26"/>
@@ -1617,7 +1696,7 @@
         <v>200</v>
       </c>
       <c r="B40" s="10" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="C40" s="11" t="n">
         <v>1</v>
@@ -1625,7 +1704,7 @@
       <c r="D40" s="12"/>
       <c r="E40" s="13"/>
       <c r="F40" s="14" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="G40" s="11"/>
       <c r="H40" s="12"/>
@@ -1638,19 +1717,19 @@
         <v>211</v>
       </c>
       <c r="B41" s="10" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="C41" s="11"/>
       <c r="D41" s="12"/>
       <c r="E41" s="13"/>
       <c r="F41" s="14" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="G41" s="11"/>
       <c r="H41" s="12"/>
       <c r="I41" s="13"/>
       <c r="J41" s="32" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="K41" s="15"/>
     </row>
@@ -1659,7 +1738,7 @@
         <v>220</v>
       </c>
       <c r="B42" s="10" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="C42" s="11" t="n">
         <v>3</v>
@@ -1667,7 +1746,7 @@
       <c r="D42" s="12"/>
       <c r="E42" s="13"/>
       <c r="F42" s="14" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="G42" s="11"/>
       <c r="H42" s="12"/>
@@ -1680,7 +1759,7 @@
         <v>230</v>
       </c>
       <c r="B43" s="10" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="C43" s="11" t="n">
         <v>3</v>
@@ -1688,7 +1767,7 @@
       <c r="D43" s="12"/>
       <c r="E43" s="13"/>
       <c r="F43" s="14" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="G43" s="11"/>
       <c r="H43" s="12"/>
@@ -1701,13 +1780,13 @@
         <v>240</v>
       </c>
       <c r="B44" s="10" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="C44" s="11"/>
       <c r="D44" s="12"/>
       <c r="E44" s="13"/>
       <c r="F44" s="14" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="G44" s="11"/>
       <c r="H44" s="12"/>
@@ -1719,7 +1798,7 @@
     </row>
     <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="34" t="s">
-        <v>64</v>
+        <v>68</v>
       </c>
       <c r="B45" s="10" t="s">
         <v>12</v>
@@ -1728,7 +1807,7 @@
       <c r="D45" s="12"/>
       <c r="E45" s="13"/>
       <c r="F45" s="14" t="s">
-        <v>65</v>
+        <v>69</v>
       </c>
       <c r="G45" s="11"/>
       <c r="H45" s="12"/>
@@ -1741,13 +1820,13 @@
         <v>250</v>
       </c>
       <c r="B46" s="10" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="C46" s="11"/>
       <c r="D46" s="12"/>
       <c r="E46" s="13"/>
       <c r="F46" s="14" t="s">
-        <v>67</v>
+        <v>71</v>
       </c>
       <c r="G46" s="11"/>
       <c r="H46" s="12"/>
@@ -1768,7 +1847,7 @@
       <c r="D47" s="12"/>
       <c r="E47" s="13"/>
       <c r="F47" s="14" t="s">
-        <v>68</v>
+        <v>72</v>
       </c>
       <c r="G47" s="11"/>
       <c r="H47" s="12"/>
@@ -1778,7 +1857,7 @@
     </row>
     <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="25" t="s">
-        <v>69</v>
+        <v>73</v>
       </c>
       <c r="B48" s="26"/>
       <c r="C48" s="26"/>
@@ -1793,10 +1872,10 @@
     </row>
     <row r="49" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="9" t="n">
-        <v>760</v>
+        <v>3060</v>
       </c>
       <c r="B49" s="10" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="C49" s="11"/>
       <c r="D49" s="12"/>
@@ -1812,16 +1891,18 @@
     </row>
     <row r="50" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="9" t="s">
-        <v>71</v>
+        <v>35</v>
       </c>
       <c r="B50" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="C50" s="11"/>
+      <c r="C50" s="11" t="s">
+        <v>35</v>
+      </c>
       <c r="D50" s="12"/>
       <c r="E50" s="13"/>
-      <c r="F50" s="14" t="s">
-        <v>71</v>
+      <c r="F50" s="14" t="n">
+        <v>44</v>
       </c>
       <c r="G50" s="11"/>
       <c r="H50" s="12"/>
@@ -1830,12 +1911,18 @@
       <c r="K50" s="15"/>
     </row>
     <row r="51" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A51" s="9"/>
-      <c r="B51" s="10"/>
+      <c r="A51" s="9" t="n">
+        <v>700</v>
+      </c>
+      <c r="B51" s="10" t="s">
+        <v>75</v>
+      </c>
       <c r="C51" s="11"/>
       <c r="D51" s="12"/>
       <c r="E51" s="13"/>
-      <c r="F51" s="14"/>
+      <c r="F51" s="14" t="s">
+        <v>35</v>
+      </c>
       <c r="G51" s="11"/>
       <c r="H51" s="12"/>
       <c r="I51" s="13"/>
@@ -1843,12 +1930,20 @@
       <c r="K51" s="15"/>
     </row>
     <row r="52" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A52" s="9"/>
-      <c r="B52" s="10"/>
-      <c r="C52" s="11"/>
+      <c r="A52" s="9" t="n">
+        <v>400</v>
+      </c>
+      <c r="B52" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="C52" s="11" t="s">
+        <v>76</v>
+      </c>
       <c r="D52" s="12"/>
       <c r="E52" s="13"/>
-      <c r="F52" s="14"/>
+      <c r="F52" s="14" t="n">
+        <v>100</v>
+      </c>
       <c r="G52" s="11"/>
       <c r="H52" s="12"/>
       <c r="I52" s="13"/>
@@ -1856,12 +1951,20 @@
       <c r="K52" s="15"/>
     </row>
     <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A53" s="9"/>
-      <c r="B53" s="10"/>
-      <c r="C53" s="11"/>
+      <c r="A53" s="9" t="n">
+        <v>400</v>
+      </c>
+      <c r="B53" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="C53" s="11" t="s">
+        <v>35</v>
+      </c>
       <c r="D53" s="12"/>
       <c r="E53" s="13"/>
-      <c r="F53" s="14"/>
+      <c r="F53" s="14" t="n">
+        <v>104</v>
+      </c>
       <c r="G53" s="11"/>
       <c r="H53" s="12"/>
       <c r="I53" s="13"/>
@@ -1869,12 +1972,18 @@
       <c r="K53" s="15"/>
     </row>
     <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A54" s="9"/>
-      <c r="B54" s="10"/>
+      <c r="A54" s="9" t="n">
+        <v>80</v>
+      </c>
+      <c r="B54" s="10" t="s">
+        <v>77</v>
+      </c>
       <c r="C54" s="11"/>
       <c r="D54" s="12"/>
       <c r="E54" s="13"/>
-      <c r="F54" s="14"/>
+      <c r="F54" s="14" t="n">
+        <v>48</v>
+      </c>
       <c r="G54" s="11"/>
       <c r="H54" s="12"/>
       <c r="I54" s="13"/>
@@ -1882,25 +1991,39 @@
       <c r="K54" s="15"/>
     </row>
     <row r="55" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A55" s="9"/>
-      <c r="B55" s="10"/>
+      <c r="A55" s="9" t="n">
+        <v>3610</v>
+      </c>
+      <c r="B55" s="10" t="s">
+        <v>78</v>
+      </c>
       <c r="C55" s="11"/>
       <c r="D55" s="12"/>
       <c r="E55" s="13"/>
-      <c r="F55" s="14"/>
+      <c r="F55" s="14" t="s">
+        <v>30</v>
+      </c>
       <c r="G55" s="11"/>
       <c r="H55" s="12"/>
       <c r="I55" s="13"/>
       <c r="J55" s="14"/>
-      <c r="K55" s="15"/>
+      <c r="K55" s="15" t="n">
+        <v>100</v>
+      </c>
     </row>
     <row r="56" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A56" s="9"/>
-      <c r="B56" s="10"/>
+      <c r="A56" s="9" t="n">
+        <v>80</v>
+      </c>
+      <c r="B56" s="10" t="s">
+        <v>12</v>
+      </c>
       <c r="C56" s="11"/>
       <c r="D56" s="12"/>
       <c r="E56" s="13"/>
-      <c r="F56" s="14"/>
+      <c r="F56" s="14" t="n">
+        <v>50</v>
+      </c>
       <c r="G56" s="11"/>
       <c r="H56" s="12"/>
       <c r="I56" s="13"/>
@@ -1908,12 +2031,18 @@
       <c r="K56" s="15"/>
     </row>
     <row r="57" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A57" s="9"/>
-      <c r="B57" s="10"/>
+      <c r="A57" s="9" t="n">
+        <v>710</v>
+      </c>
+      <c r="B57" s="10" t="s">
+        <v>79</v>
+      </c>
       <c r="C57" s="11"/>
       <c r="D57" s="12"/>
       <c r="E57" s="13"/>
-      <c r="F57" s="14"/>
+      <c r="F57" s="14" t="n">
+        <v>100</v>
+      </c>
       <c r="G57" s="11"/>
       <c r="H57" s="12"/>
       <c r="I57" s="13"/>
@@ -1921,12 +2050,20 @@
       <c r="K57" s="15"/>
     </row>
     <row r="58" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A58" s="9"/>
-      <c r="B58" s="10"/>
-      <c r="C58" s="11"/>
+      <c r="A58" s="9" t="n">
+        <v>400</v>
+      </c>
+      <c r="B58" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="C58" s="11" t="s">
+        <v>76</v>
+      </c>
       <c r="D58" s="12"/>
       <c r="E58" s="13"/>
-      <c r="F58" s="14"/>
+      <c r="F58" s="14" t="n">
+        <v>104</v>
+      </c>
       <c r="G58" s="11"/>
       <c r="H58" s="12"/>
       <c r="I58" s="13"/>
@@ -1934,90 +2071,142 @@
       <c r="K58" s="15"/>
     </row>
     <row r="59" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A59" s="9"/>
-      <c r="B59" s="10"/>
+      <c r="A59" s="9" t="n">
+        <v>80</v>
+      </c>
+      <c r="B59" s="10" t="s">
+        <v>77</v>
+      </c>
       <c r="C59" s="11"/>
       <c r="D59" s="12"/>
       <c r="E59" s="13"/>
-      <c r="F59" s="14"/>
+      <c r="F59" s="14" t="n">
+        <v>54</v>
+      </c>
       <c r="G59" s="11"/>
       <c r="H59" s="12"/>
       <c r="I59" s="13"/>
       <c r="J59" s="14"/>
       <c r="K59" s="15"/>
     </row>
-    <row r="60" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A60" s="9"/>
-      <c r="B60" s="10"/>
-      <c r="C60" s="11"/>
+    <row r="60" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A60" s="9" t="n">
+        <v>400</v>
+      </c>
+      <c r="B60" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="C60" s="11" t="s">
+        <v>35</v>
+      </c>
       <c r="D60" s="12"/>
       <c r="E60" s="13"/>
-      <c r="F60" s="14"/>
+      <c r="F60" s="14" t="n">
+        <v>58</v>
+      </c>
       <c r="G60" s="11"/>
       <c r="H60" s="12"/>
       <c r="I60" s="13"/>
       <c r="J60" s="14"/>
       <c r="K60" s="15"/>
     </row>
-    <row r="61" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A61" s="9"/>
-      <c r="B61" s="10"/>
-      <c r="C61" s="11"/>
+    <row r="61" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A61" s="9" t="n">
+        <v>720</v>
+      </c>
+      <c r="B61" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="C61" s="11" t="s">
+        <v>81</v>
+      </c>
       <c r="D61" s="12"/>
       <c r="E61" s="13"/>
-      <c r="F61" s="14"/>
+      <c r="F61" s="14" t="s">
+        <v>35</v>
+      </c>
       <c r="G61" s="11"/>
       <c r="H61" s="12"/>
       <c r="I61" s="13"/>
       <c r="J61" s="14"/>
       <c r="K61" s="15"/>
     </row>
-    <row r="62" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A62" s="9"/>
-      <c r="B62" s="10"/>
-      <c r="C62" s="11"/>
+    <row r="62" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A62" s="9" t="n">
+        <v>400</v>
+      </c>
+      <c r="B62" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="C62" s="11" t="s">
+        <v>82</v>
+      </c>
       <c r="D62" s="12"/>
       <c r="E62" s="13"/>
-      <c r="F62" s="14"/>
+      <c r="F62" s="14" t="n">
+        <v>100</v>
+      </c>
       <c r="G62" s="11"/>
       <c r="H62" s="12"/>
       <c r="I62" s="13"/>
       <c r="J62" s="14"/>
       <c r="K62" s="15"/>
     </row>
-    <row r="63" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A63" s="9"/>
-      <c r="B63" s="10"/>
-      <c r="C63" s="11"/>
+    <row r="63" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A63" s="9" t="n">
+        <v>400</v>
+      </c>
+      <c r="B63" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="C63" s="11" t="s">
+        <v>81</v>
+      </c>
       <c r="D63" s="12"/>
       <c r="E63" s="13"/>
-      <c r="F63" s="14"/>
+      <c r="F63" s="14" t="n">
+        <v>104</v>
+      </c>
       <c r="G63" s="11"/>
       <c r="H63" s="12"/>
       <c r="I63" s="13"/>
       <c r="J63" s="14"/>
       <c r="K63" s="15"/>
     </row>
-    <row r="64" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A64" s="9"/>
-      <c r="B64" s="10"/>
+    <row r="64" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A64" s="9" t="n">
+        <v>80</v>
+      </c>
+      <c r="B64" s="10" t="s">
+        <v>77</v>
+      </c>
       <c r="C64" s="11"/>
       <c r="D64" s="12"/>
       <c r="E64" s="13"/>
-      <c r="F64" s="14"/>
+      <c r="F64" s="14" t="s">
+        <v>36</v>
+      </c>
       <c r="G64" s="11"/>
       <c r="H64" s="12"/>
       <c r="I64" s="13"/>
       <c r="J64" s="14"/>
       <c r="K64" s="15"/>
     </row>
-    <row r="65" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A65" s="9"/>
-      <c r="B65" s="10"/>
-      <c r="C65" s="11"/>
+    <row r="65" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A65" s="9" t="n">
+        <v>730</v>
+      </c>
+      <c r="B65" s="10" t="s">
+        <v>83</v>
+      </c>
+      <c r="C65" s="11" t="s">
+        <v>35</v>
+      </c>
       <c r="D65" s="12"/>
       <c r="E65" s="13"/>
-      <c r="F65" s="14"/>
+      <c r="F65" s="14" t="s">
+        <v>35</v>
+      </c>
       <c r="G65" s="11"/>
       <c r="H65" s="12"/>
       <c r="I65" s="13"/>
@@ -2025,44 +2214,337 @@
       <c r="K65" s="15"/>
     </row>
     <row r="66" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A66" s="9"/>
-      <c r="B66" s="10"/>
-      <c r="C66" s="11"/>
+      <c r="A66" s="9" t="n">
+        <v>400</v>
+      </c>
+      <c r="B66" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="C66" s="11" t="s">
+        <v>76</v>
+      </c>
       <c r="D66" s="12"/>
       <c r="E66" s="13"/>
-      <c r="F66" s="14"/>
+      <c r="F66" s="14" t="n">
+        <v>100</v>
+      </c>
       <c r="G66" s="11"/>
       <c r="H66" s="12"/>
       <c r="I66" s="13"/>
       <c r="J66" s="14"/>
       <c r="K66" s="15"/>
     </row>
-    <row r="67" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A67" s="9"/>
-      <c r="B67" s="10"/>
-      <c r="C67" s="11"/>
+    <row r="67" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A67" s="9" t="n">
+        <v>400</v>
+      </c>
+      <c r="B67" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="C67" s="11" t="s">
+        <v>35</v>
+      </c>
       <c r="D67" s="12"/>
       <c r="E67" s="13"/>
-      <c r="F67" s="14"/>
+      <c r="F67" s="14" t="n">
+        <v>104</v>
+      </c>
       <c r="G67" s="11"/>
       <c r="H67" s="12"/>
       <c r="I67" s="13"/>
       <c r="J67" s="14"/>
       <c r="K67" s="15"/>
     </row>
-    <row r="68" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A68" s="35"/>
-      <c r="B68" s="36"/>
+    <row r="68" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A68" s="35" t="n">
+        <v>80</v>
+      </c>
+      <c r="B68" s="36" t="s">
+        <v>77</v>
+      </c>
       <c r="C68" s="37"/>
       <c r="D68" s="38"/>
       <c r="E68" s="39"/>
-      <c r="F68" s="40"/>
+      <c r="F68" s="40" t="n">
+        <v>60</v>
+      </c>
       <c r="G68" s="37"/>
       <c r="H68" s="38"/>
       <c r="I68" s="39"/>
       <c r="J68" s="40"/>
       <c r="K68" s="41"/>
     </row>
+    <row r="69" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A69" s="9" t="n">
+        <v>740</v>
+      </c>
+      <c r="B69" s="10" t="s">
+        <v>84</v>
+      </c>
+      <c r="C69" s="11"/>
+      <c r="D69" s="12"/>
+      <c r="E69" s="13"/>
+      <c r="F69" s="14" t="n">
+        <v>100</v>
+      </c>
+      <c r="G69" s="11"/>
+      <c r="H69" s="12"/>
+      <c r="I69" s="13"/>
+      <c r="J69" s="14"/>
+      <c r="K69" s="15"/>
+    </row>
+    <row r="70" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A70" s="35" t="n">
+        <v>4</v>
+      </c>
+      <c r="B70" s="36" t="s">
+        <v>12</v>
+      </c>
+      <c r="C70" s="37"/>
+      <c r="D70" s="38"/>
+      <c r="E70" s="39"/>
+      <c r="F70" s="40"/>
+      <c r="G70" s="37"/>
+      <c r="H70" s="38"/>
+      <c r="I70" s="39"/>
+      <c r="J70" s="40"/>
+      <c r="K70" s="41"/>
+    </row>
+    <row r="71" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A71" s="9" t="n">
+        <v>400</v>
+      </c>
+      <c r="B71" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="C71" s="11" t="s">
+        <v>76</v>
+      </c>
+      <c r="D71" s="12"/>
+      <c r="E71" s="13"/>
+      <c r="F71" s="14" t="n">
+        <v>104</v>
+      </c>
+      <c r="G71" s="11"/>
+      <c r="H71" s="12"/>
+      <c r="I71" s="13"/>
+      <c r="J71" s="14"/>
+      <c r="K71" s="15"/>
+    </row>
+    <row r="72" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A72" s="35" t="n">
+        <v>80</v>
+      </c>
+      <c r="B72" s="36" t="s">
+        <v>77</v>
+      </c>
+      <c r="C72" s="37"/>
+      <c r="D72" s="38"/>
+      <c r="E72" s="39"/>
+      <c r="F72" s="40" t="n">
+        <v>68</v>
+      </c>
+      <c r="G72" s="37"/>
+      <c r="H72" s="38"/>
+      <c r="I72" s="39"/>
+      <c r="J72" s="40"/>
+      <c r="K72" s="41"/>
+    </row>
+    <row r="73" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A73" s="9" t="n">
+        <v>750</v>
+      </c>
+      <c r="B73" s="10" t="s">
+        <v>85</v>
+      </c>
+      <c r="C73" s="11"/>
+      <c r="D73" s="12"/>
+      <c r="E73" s="13"/>
+      <c r="F73" s="14" t="n">
+        <v>108</v>
+      </c>
+      <c r="G73" s="11"/>
+      <c r="H73" s="12"/>
+      <c r="I73" s="13"/>
+      <c r="J73" s="14"/>
+      <c r="K73" s="15"/>
+    </row>
+    <row r="74" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A74" s="35" t="n">
+        <v>108</v>
+      </c>
+      <c r="B74" s="36" t="s">
+        <v>12</v>
+      </c>
+      <c r="C74" s="37"/>
+      <c r="D74" s="38"/>
+      <c r="E74" s="39"/>
+      <c r="F74" s="40"/>
+      <c r="G74" s="37"/>
+      <c r="H74" s="38"/>
+      <c r="I74" s="39"/>
+      <c r="J74" s="40"/>
+      <c r="K74" s="41"/>
+    </row>
+    <row r="75" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A75" s="9" t="n">
+        <v>400</v>
+      </c>
+      <c r="B75" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="C75" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="D75" s="12"/>
+      <c r="E75" s="13"/>
+      <c r="F75" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="G75" s="11"/>
+      <c r="H75" s="12"/>
+      <c r="I75" s="13"/>
+      <c r="J75" s="14"/>
+      <c r="K75" s="15"/>
+    </row>
+    <row r="76" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A76" s="35" t="n">
+        <v>80</v>
+      </c>
+      <c r="B76" s="36" t="s">
+        <v>77</v>
+      </c>
+      <c r="C76" s="37"/>
+      <c r="D76" s="38"/>
+      <c r="E76" s="39"/>
+      <c r="F76" s="40" t="n">
+        <v>70</v>
+      </c>
+      <c r="G76" s="37"/>
+      <c r="H76" s="38"/>
+      <c r="I76" s="39"/>
+      <c r="J76" s="40"/>
+      <c r="K76" s="41"/>
+    </row>
+    <row r="77" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A77" s="9"/>
+      <c r="B77" s="10"/>
+      <c r="C77" s="11"/>
+      <c r="D77" s="12"/>
+      <c r="E77" s="13"/>
+      <c r="F77" s="14"/>
+      <c r="G77" s="11"/>
+      <c r="H77" s="12"/>
+      <c r="I77" s="13"/>
+      <c r="J77" s="14"/>
+      <c r="K77" s="15"/>
+    </row>
+    <row r="78" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A78" s="35"/>
+      <c r="B78" s="36"/>
+      <c r="C78" s="37"/>
+      <c r="D78" s="38"/>
+      <c r="E78" s="39"/>
+      <c r="F78" s="40"/>
+      <c r="G78" s="37"/>
+      <c r="H78" s="38"/>
+      <c r="I78" s="39"/>
+      <c r="J78" s="40"/>
+      <c r="K78" s="41"/>
+    </row>
+    <row r="79" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A79" s="9"/>
+      <c r="B79" s="10"/>
+      <c r="C79" s="11"/>
+      <c r="D79" s="12"/>
+      <c r="E79" s="13"/>
+      <c r="F79" s="14"/>
+      <c r="G79" s="11"/>
+      <c r="H79" s="12"/>
+      <c r="I79" s="13"/>
+      <c r="J79" s="14"/>
+      <c r="K79" s="15"/>
+    </row>
+    <row r="80" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A80" s="35"/>
+      <c r="B80" s="36"/>
+      <c r="C80" s="37"/>
+      <c r="D80" s="38"/>
+      <c r="E80" s="39"/>
+      <c r="F80" s="40"/>
+      <c r="G80" s="37"/>
+      <c r="H80" s="38"/>
+      <c r="I80" s="39"/>
+      <c r="J80" s="40"/>
+      <c r="K80" s="41"/>
+    </row>
+    <row r="81" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A81" s="9"/>
+      <c r="B81" s="10"/>
+      <c r="C81" s="11"/>
+      <c r="D81" s="12"/>
+      <c r="E81" s="13"/>
+      <c r="F81" s="14"/>
+      <c r="G81" s="11"/>
+      <c r="H81" s="12"/>
+      <c r="I81" s="13"/>
+      <c r="J81" s="14"/>
+      <c r="K81" s="15"/>
+    </row>
+    <row r="82" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A82" s="35"/>
+      <c r="B82" s="36"/>
+      <c r="C82" s="37"/>
+      <c r="D82" s="38"/>
+      <c r="E82" s="39"/>
+      <c r="F82" s="40"/>
+      <c r="G82" s="37"/>
+      <c r="H82" s="38"/>
+      <c r="I82" s="39"/>
+      <c r="J82" s="40"/>
+      <c r="K82" s="41"/>
+    </row>
+    <row r="83" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A83" s="9"/>
+      <c r="B83" s="10"/>
+      <c r="C83" s="11"/>
+      <c r="D83" s="12"/>
+      <c r="E83" s="13"/>
+      <c r="F83" s="14"/>
+      <c r="G83" s="11"/>
+      <c r="H83" s="12"/>
+      <c r="I83" s="13"/>
+      <c r="J83" s="14"/>
+      <c r="K83" s="15"/>
+    </row>
+    <row r="84" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A84" s="35"/>
+      <c r="B84" s="36"/>
+      <c r="C84" s="37"/>
+      <c r="D84" s="38"/>
+      <c r="E84" s="39"/>
+      <c r="F84" s="40"/>
+      <c r="G84" s="37"/>
+      <c r="H84" s="38"/>
+      <c r="I84" s="39"/>
+      <c r="J84" s="40"/>
+      <c r="K84" s="41"/>
+    </row>
+    <row r="85" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A85" s="9"/>
+      <c r="B85" s="10"/>
+      <c r="C85" s="11"/>
+      <c r="D85" s="12"/>
+      <c r="E85" s="13"/>
+      <c r="F85" s="14"/>
+      <c r="G85" s="11"/>
+      <c r="H85" s="12"/>
+      <c r="I85" s="13"/>
+      <c r="J85" s="14"/>
+      <c r="K85" s="15"/>
+    </row>
+    <row r="86" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="87" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>

</xml_diff>